<commit_message>
Renamed Haven ChunkType to Chromatic Conondrum
</commit_message>
<xml_diff>
--- a/BiomeMap.xlsx
+++ b/BiomeMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Projects\Unity Projects\Terror of Infinity - Thesis Edition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912AD2C3-64C9-492B-ADC9-A0B5BD2C7059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05131997-5E5F-4B1A-8152-09F3AD97C27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2655" windowWidth="24240" windowHeight="13140" xr2:uid="{7D3A4204-C59A-488D-A1E0-BAE9CFBB8776}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D3A4204-C59A-488D-A1E0-BAE9CFBB8776}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>BLACK</t>
   </si>
@@ -187,9 +187,6 @@
 the Darkness moves by a Light during a Hunt, the Hunt ends.</t>
   </si>
   <si>
-    <t>Haven</t>
-  </si>
-  <si>
     <t>The Bright of Angels</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t>DEATH IMPLEMENTATION REQ</t>
+  </si>
+  <si>
+    <t>Chromatic Conondrum</t>
+  </si>
+  <si>
+    <t>Chromatic Conundrum</t>
   </si>
 </sst>
 </file>
@@ -672,6 +675,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -681,13 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,17 +1038,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>52</v>
+      <c r="A1" s="76" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
+      <c r="A2" s="77"/>
     </row>
     <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
+      <c r="A3" s="77"/>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1055,7 +1058,7 @@
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
@@ -1067,46 +1070,46 @@
       </c>
       <c r="P3" s="6"/>
       <c r="R3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC3" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC3" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="AD3" s="76"/>
-      <c r="AE3" s="76"/>
-      <c r="AG3" s="76" t="s">
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="74"/>
+      <c r="AG3" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="77"/>
-      <c r="AI3" s="77"/>
-      <c r="AK3" s="76" t="s">
+      <c r="AH3" s="75"/>
+      <c r="AI3" s="75"/>
+      <c r="AK3" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="AL3" s="76"/>
-      <c r="AM3" s="76"/>
+      <c r="AL3" s="74"/>
+      <c r="AM3" s="74"/>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
+      <c r="A4" s="77"/>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>0.9</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="I4" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M4" s="42"/>
       <c r="O4" s="49" t="s">
@@ -1114,20 +1117,20 @@
       </c>
       <c r="P4" s="6"/>
       <c r="R4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC4" s="76"/>
-      <c r="AD4" s="76"/>
-      <c r="AE4" s="76"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="77"/>
-      <c r="AK4" s="76"/>
-      <c r="AL4" s="76"/>
-      <c r="AM4" s="76"/>
+        <v>60</v>
+      </c>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AG4" s="75"/>
+      <c r="AH4" s="75"/>
+      <c r="AI4" s="75"/>
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="74"/>
+      <c r="A5" s="77"/>
       <c r="B5" t="s">
         <v>33</v>
       </c>
@@ -1155,20 +1158,20 @@
       </c>
       <c r="P5" s="6"/>
       <c r="R5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC5" s="76"/>
-      <c r="AD5" s="76"/>
-      <c r="AE5" s="76"/>
-      <c r="AG5" s="77"/>
-      <c r="AH5" s="77"/>
-      <c r="AI5" s="77"/>
-      <c r="AK5" s="76"/>
-      <c r="AL5" s="76"/>
-      <c r="AM5" s="76"/>
+        <v>61</v>
+      </c>
+      <c r="AC5" s="74"/>
+      <c r="AD5" s="74"/>
+      <c r="AE5" s="74"/>
+      <c r="AG5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AK5" s="74"/>
+      <c r="AL5" s="74"/>
+      <c r="AM5" s="74"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
+      <c r="A6" s="77"/>
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1178,32 +1181,32 @@
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="39" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="O6" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="76"/>
-      <c r="AD6" s="76"/>
-      <c r="AE6" s="76"/>
-      <c r="AG6" s="77"/>
-      <c r="AH6" s="77"/>
-      <c r="AI6" s="77"/>
-      <c r="AK6" s="76"/>
-      <c r="AL6" s="76"/>
-      <c r="AM6" s="76"/>
+      <c r="AC6" s="74"/>
+      <c r="AD6" s="74"/>
+      <c r="AE6" s="74"/>
+      <c r="AG6" s="75"/>
+      <c r="AH6" s="75"/>
+      <c r="AI6" s="75"/>
+      <c r="AK6" s="74"/>
+      <c r="AL6" s="74"/>
+      <c r="AM6" s="74"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
+      <c r="A7" s="77"/>
       <c r="B7" t="s">
         <v>29</v>
       </c>
@@ -1229,20 +1232,20 @@
       </c>
       <c r="P7" s="6"/>
       <c r="R7" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC7" s="76"/>
-      <c r="AD7" s="76"/>
-      <c r="AE7" s="76"/>
-      <c r="AG7" s="77"/>
-      <c r="AH7" s="77"/>
-      <c r="AI7" s="77"/>
-      <c r="AK7" s="76"/>
-      <c r="AL7" s="76"/>
-      <c r="AM7" s="76"/>
+        <v>62</v>
+      </c>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AG7" s="75"/>
+      <c r="AH7" s="75"/>
+      <c r="AI7" s="75"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="74"/>
+      <c r="AM7" s="74"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="74"/>
+      <c r="A8" s="77"/>
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1268,20 +1271,20 @@
       </c>
       <c r="P8" s="6"/>
       <c r="R8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC8" s="76"/>
-      <c r="AD8" s="76"/>
-      <c r="AE8" s="76"/>
-      <c r="AG8" s="77"/>
-      <c r="AH8" s="77"/>
-      <c r="AI8" s="77"/>
-      <c r="AK8" s="76"/>
-      <c r="AL8" s="76"/>
-      <c r="AM8" s="76"/>
+        <v>63</v>
+      </c>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AG8" s="75"/>
+      <c r="AH8" s="75"/>
+      <c r="AI8" s="75"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="74"/>
+      <c r="A9" s="77"/>
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>0.4</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
@@ -1300,7 +1303,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="10"/>
       <c r="K9" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -1309,23 +1312,23 @@
       </c>
       <c r="P9" s="72"/>
       <c r="Q9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC9" s="76"/>
-      <c r="AD9" s="76"/>
-      <c r="AE9" s="76"/>
-      <c r="AG9" s="77"/>
-      <c r="AH9" s="77"/>
-      <c r="AI9" s="77"/>
-      <c r="AK9" s="76"/>
-      <c r="AL9" s="76"/>
-      <c r="AM9" s="76"/>
+        <v>64</v>
+      </c>
+      <c r="AC9" s="74"/>
+      <c r="AD9" s="74"/>
+      <c r="AE9" s="74"/>
+      <c r="AG9" s="75"/>
+      <c r="AH9" s="75"/>
+      <c r="AI9" s="75"/>
+      <c r="AK9" s="74"/>
+      <c r="AL9" s="74"/>
+      <c r="AM9" s="74"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="74"/>
+      <c r="A10" s="77"/>
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1335,7 +1338,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -1349,27 +1352,27 @@
       </c>
       <c r="M10" s="32"/>
       <c r="O10" s="54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P10" s="6"/>
       <c r="Q10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC10" s="76"/>
-      <c r="AD10" s="76"/>
-      <c r="AE10" s="76"/>
-      <c r="AG10" s="77"/>
-      <c r="AH10" s="77"/>
-      <c r="AI10" s="77"/>
-      <c r="AK10" s="76"/>
-      <c r="AL10" s="76"/>
-      <c r="AM10" s="76"/>
+        <v>65</v>
+      </c>
+      <c r="AC10" s="74"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
+      <c r="AG10" s="75"/>
+      <c r="AH10" s="75"/>
+      <c r="AI10" s="75"/>
+      <c r="AK10" s="74"/>
+      <c r="AL10" s="74"/>
+      <c r="AM10" s="74"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="74"/>
+      <c r="A11" s="77"/>
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -1391,20 +1394,20 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="O11" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC11" s="76"/>
-      <c r="AD11" s="76"/>
-      <c r="AE11" s="76"/>
-      <c r="AG11" s="77"/>
-      <c r="AH11" s="77"/>
-      <c r="AI11" s="77"/>
-      <c r="AK11" s="76"/>
-      <c r="AL11" s="76"/>
-      <c r="AM11" s="76"/>
+        <v>59</v>
+      </c>
+      <c r="AC11" s="74"/>
+      <c r="AD11" s="74"/>
+      <c r="AE11" s="74"/>
+      <c r="AG11" s="75"/>
+      <c r="AH11" s="75"/>
+      <c r="AI11" s="75"/>
+      <c r="AK11" s="74"/>
+      <c r="AL11" s="74"/>
+      <c r="AM11" s="74"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
+      <c r="A12" s="77"/>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -1424,7 +1427,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="27"/>
       <c r="L12" s="27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M12" s="2"/>
       <c r="O12" s="56" t="s">
@@ -1432,20 +1435,20 @@
       </c>
       <c r="P12" s="6"/>
       <c r="R12" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC12" s="76"/>
-      <c r="AD12" s="76"/>
-      <c r="AE12" s="76"/>
-      <c r="AG12" s="77"/>
-      <c r="AH12" s="77"/>
-      <c r="AI12" s="77"/>
-      <c r="AK12" s="76"/>
-      <c r="AL12" s="76"/>
-      <c r="AM12" s="76"/>
+        <v>66</v>
+      </c>
+      <c r="AC12" s="74"/>
+      <c r="AD12" s="74"/>
+      <c r="AE12" s="74"/>
+      <c r="AG12" s="75"/>
+      <c r="AH12" s="75"/>
+      <c r="AI12" s="75"/>
+      <c r="AK12" s="74"/>
+      <c r="AL12" s="74"/>
+      <c r="AM12" s="74"/>
     </row>
     <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74"/>
+      <c r="A13" s="77"/>
       <c r="C13">
         <v>0</v>
       </c>
@@ -1480,15 +1483,15 @@
         <v>1</v>
       </c>
       <c r="O13" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P13" s="6"/>
       <c r="R13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
+      <c r="A14" s="77"/>
       <c r="D14" t="s">
         <v>0</v>
       </c>
@@ -1524,84 +1527,84 @@
       </c>
       <c r="P14" s="6"/>
       <c r="R14" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC14" s="76" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD14" s="76"/>
-      <c r="AE14" s="76"/>
-      <c r="AG14" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC14" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD14" s="74"/>
+      <c r="AE14" s="74"/>
+      <c r="AG14" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="AH14" s="76"/>
-      <c r="AI14" s="76"/>
-      <c r="AK14" s="76" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL14" s="76"/>
-      <c r="AM14" s="76"/>
+      <c r="AH14" s="74"/>
+      <c r="AI14" s="74"/>
+      <c r="AK14" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL14" s="74"/>
+      <c r="AM14" s="74"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="C15" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
+      <c r="A15" s="77"/>
+      <c r="C15" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
       <c r="O15" s="59" t="s">
         <v>28</v>
       </c>
       <c r="P15" s="6"/>
       <c r="R15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC15" s="76"/>
-      <c r="AD15" s="76"/>
-      <c r="AE15" s="76"/>
-      <c r="AG15" s="76"/>
-      <c r="AH15" s="76"/>
-      <c r="AI15" s="76"/>
-      <c r="AK15" s="76"/>
-      <c r="AL15" s="76"/>
-      <c r="AM15" s="76"/>
+        <v>69</v>
+      </c>
+      <c r="AC15" s="74"/>
+      <c r="AD15" s="74"/>
+      <c r="AE15" s="74"/>
+      <c r="AG15" s="74"/>
+      <c r="AH15" s="74"/>
+      <c r="AI15" s="74"/>
+      <c r="AK15" s="74"/>
+      <c r="AL15" s="74"/>
+      <c r="AM15" s="74"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
       <c r="O16" s="60" t="s">
         <v>31</v>
       </c>
       <c r="P16" s="6"/>
       <c r="R16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC16" s="76"/>
-      <c r="AD16" s="76"/>
-      <c r="AE16" s="76"/>
-      <c r="AG16" s="76"/>
-      <c r="AH16" s="76"/>
-      <c r="AI16" s="76"/>
-      <c r="AK16" s="76"/>
-      <c r="AL16" s="76"/>
-      <c r="AM16" s="76"/>
+        <v>70</v>
+      </c>
+      <c r="AC16" s="74"/>
+      <c r="AD16" s="74"/>
+      <c r="AE16" s="74"/>
+      <c r="AG16" s="74"/>
+      <c r="AH16" s="74"/>
+      <c r="AI16" s="74"/>
+      <c r="AK16" s="74"/>
+      <c r="AL16" s="74"/>
+      <c r="AM16" s="74"/>
     </row>
     <row r="17" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O17" s="61" t="s">
@@ -1609,294 +1612,299 @@
       </c>
       <c r="P17" s="72"/>
       <c r="R17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="76"/>
-      <c r="AE17" s="76"/>
-      <c r="AG17" s="76"/>
-      <c r="AH17" s="76"/>
-      <c r="AI17" s="76"/>
-      <c r="AK17" s="76"/>
-      <c r="AL17" s="76"/>
-      <c r="AM17" s="76"/>
+        <v>71</v>
+      </c>
+      <c r="AC17" s="74"/>
+      <c r="AD17" s="74"/>
+      <c r="AE17" s="74"/>
+      <c r="AG17" s="74"/>
+      <c r="AH17" s="74"/>
+      <c r="AI17" s="74"/>
+      <c r="AK17" s="74"/>
+      <c r="AL17" s="74"/>
+      <c r="AM17" s="74"/>
     </row>
     <row r="18" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O18" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="AC18" s="76"/>
-      <c r="AD18" s="76"/>
-      <c r="AE18" s="76"/>
-      <c r="AG18" s="76"/>
-      <c r="AH18" s="76"/>
-      <c r="AI18" s="76"/>
-      <c r="AK18" s="76"/>
-      <c r="AL18" s="76"/>
-      <c r="AM18" s="76"/>
+      <c r="AC18" s="74"/>
+      <c r="AD18" s="74"/>
+      <c r="AE18" s="74"/>
+      <c r="AG18" s="74"/>
+      <c r="AH18" s="74"/>
+      <c r="AI18" s="74"/>
+      <c r="AK18" s="74"/>
+      <c r="AL18" s="74"/>
+      <c r="AM18" s="74"/>
     </row>
     <row r="19" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O19" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="76"/>
-      <c r="AE19" s="76"/>
-      <c r="AG19" s="76"/>
-      <c r="AH19" s="76"/>
-      <c r="AI19" s="76"/>
-      <c r="AK19" s="76"/>
-      <c r="AL19" s="76"/>
-      <c r="AM19" s="76"/>
+      <c r="AC19" s="74"/>
+      <c r="AD19" s="74"/>
+      <c r="AE19" s="74"/>
+      <c r="AG19" s="74"/>
+      <c r="AH19" s="74"/>
+      <c r="AI19" s="74"/>
+      <c r="AK19" s="74"/>
+      <c r="AL19" s="74"/>
+      <c r="AM19" s="74"/>
     </row>
     <row r="20" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O20" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="AC20" s="76"/>
-      <c r="AD20" s="76"/>
-      <c r="AE20" s="76"/>
-      <c r="AG20" s="76"/>
-      <c r="AH20" s="76"/>
-      <c r="AI20" s="76"/>
-      <c r="AK20" s="76"/>
-      <c r="AL20" s="76"/>
-      <c r="AM20" s="76"/>
+      <c r="AC20" s="74"/>
+      <c r="AD20" s="74"/>
+      <c r="AE20" s="74"/>
+      <c r="AG20" s="74"/>
+      <c r="AH20" s="74"/>
+      <c r="AI20" s="74"/>
+      <c r="AK20" s="74"/>
+      <c r="AL20" s="74"/>
+      <c r="AM20" s="74"/>
     </row>
     <row r="21" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O21" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="P21" s="78"/>
+        <v>76</v>
+      </c>
+      <c r="P21" s="73"/>
       <c r="Q21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC21" s="76"/>
-      <c r="AD21" s="76"/>
-      <c r="AE21" s="76"/>
-      <c r="AG21" s="76"/>
-      <c r="AH21" s="76"/>
-      <c r="AI21" s="76"/>
-      <c r="AK21" s="76"/>
-      <c r="AL21" s="76"/>
-      <c r="AM21" s="76"/>
+        <v>74</v>
+      </c>
+      <c r="AC21" s="74"/>
+      <c r="AD21" s="74"/>
+      <c r="AE21" s="74"/>
+      <c r="AG21" s="74"/>
+      <c r="AH21" s="74"/>
+      <c r="AI21" s="74"/>
+      <c r="AK21" s="74"/>
+      <c r="AL21" s="74"/>
+      <c r="AM21" s="74"/>
     </row>
     <row r="22" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O22" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC22" s="76"/>
-      <c r="AD22" s="76"/>
-      <c r="AE22" s="76"/>
-      <c r="AG22" s="76"/>
-      <c r="AH22" s="76"/>
-      <c r="AI22" s="76"/>
-      <c r="AK22" s="76"/>
-      <c r="AL22" s="76"/>
-      <c r="AM22" s="76"/>
+        <v>40</v>
+      </c>
+      <c r="AC22" s="74"/>
+      <c r="AD22" s="74"/>
+      <c r="AE22" s="74"/>
+      <c r="AG22" s="74"/>
+      <c r="AH22" s="74"/>
+      <c r="AI22" s="74"/>
+      <c r="AK22" s="74"/>
+      <c r="AL22" s="74"/>
+      <c r="AM22" s="74"/>
     </row>
     <row r="23" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O23" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC23" s="76"/>
-      <c r="AD23" s="76"/>
-      <c r="AE23" s="76"/>
-      <c r="AG23" s="76"/>
-      <c r="AH23" s="76"/>
-      <c r="AI23" s="76"/>
-      <c r="AK23" s="76"/>
-      <c r="AL23" s="76"/>
-      <c r="AM23" s="76"/>
+        <v>43</v>
+      </c>
+      <c r="AC23" s="74"/>
+      <c r="AD23" s="74"/>
+      <c r="AE23" s="74"/>
+      <c r="AG23" s="74"/>
+      <c r="AH23" s="74"/>
+      <c r="AI23" s="74"/>
+      <c r="AK23" s="74"/>
+      <c r="AL23" s="74"/>
+      <c r="AM23" s="74"/>
     </row>
     <row r="24" spans="15:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O24" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="15:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O25" s="69" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="R25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC25" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC25" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="AD25" s="76"/>
-      <c r="AE25" s="76"/>
-      <c r="AG25" s="76" t="s">
+      <c r="AD25" s="74"/>
+      <c r="AE25" s="74"/>
+      <c r="AG25" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="AH25" s="76"/>
-      <c r="AI25" s="76"/>
-      <c r="AK25" s="76" t="s">
+      <c r="AH25" s="74"/>
+      <c r="AI25" s="74"/>
+      <c r="AK25" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="AL25" s="76"/>
-      <c r="AM25" s="76"/>
+      <c r="AL25" s="74"/>
+      <c r="AM25" s="74"/>
     </row>
     <row r="26" spans="15:39" x14ac:dyDescent="0.25">
       <c r="O26" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC26" s="74"/>
+      <c r="AD26" s="74"/>
+      <c r="AE26" s="74"/>
+      <c r="AG26" s="74"/>
+      <c r="AH26" s="74"/>
+      <c r="AI26" s="74"/>
+      <c r="AK26" s="74"/>
+      <c r="AL26" s="74"/>
+      <c r="AM26" s="74"/>
+    </row>
+    <row r="27" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC27" s="74"/>
+      <c r="AD27" s="74"/>
+      <c r="AE27" s="74"/>
+      <c r="AG27" s="74"/>
+      <c r="AH27" s="74"/>
+      <c r="AI27" s="74"/>
+      <c r="AK27" s="74"/>
+      <c r="AL27" s="74"/>
+      <c r="AM27" s="74"/>
+    </row>
+    <row r="28" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC28" s="74"/>
+      <c r="AD28" s="74"/>
+      <c r="AE28" s="74"/>
+      <c r="AG28" s="74"/>
+      <c r="AH28" s="74"/>
+      <c r="AI28" s="74"/>
+      <c r="AK28" s="74"/>
+      <c r="AL28" s="74"/>
+      <c r="AM28" s="74"/>
+    </row>
+    <row r="29" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="74"/>
+      <c r="AE29" s="74"/>
+      <c r="AG29" s="74"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="74"/>
+      <c r="AK29" s="74"/>
+      <c r="AL29" s="74"/>
+      <c r="AM29" s="74"/>
+    </row>
+    <row r="30" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC30" s="74"/>
+      <c r="AD30" s="74"/>
+      <c r="AE30" s="74"/>
+      <c r="AG30" s="74"/>
+      <c r="AH30" s="74"/>
+      <c r="AI30" s="74"/>
+      <c r="AK30" s="74"/>
+      <c r="AL30" s="74"/>
+      <c r="AM30" s="74"/>
+    </row>
+    <row r="31" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC31" s="74"/>
+      <c r="AD31" s="74"/>
+      <c r="AE31" s="74"/>
+      <c r="AG31" s="74"/>
+      <c r="AH31" s="74"/>
+      <c r="AI31" s="74"/>
+      <c r="AK31" s="74"/>
+      <c r="AL31" s="74"/>
+      <c r="AM31" s="74"/>
+    </row>
+    <row r="32" spans="15:39" x14ac:dyDescent="0.25">
+      <c r="AC32" s="74"/>
+      <c r="AD32" s="74"/>
+      <c r="AE32" s="74"/>
+      <c r="AG32" s="74"/>
+      <c r="AH32" s="74"/>
+      <c r="AI32" s="74"/>
+      <c r="AK32" s="74"/>
+      <c r="AL32" s="74"/>
+      <c r="AM32" s="74"/>
+    </row>
+    <row r="33" spans="29:39" x14ac:dyDescent="0.25">
+      <c r="AC33" s="74"/>
+      <c r="AD33" s="74"/>
+      <c r="AE33" s="74"/>
+      <c r="AG33" s="74"/>
+      <c r="AH33" s="74"/>
+      <c r="AI33" s="74"/>
+      <c r="AK33" s="74"/>
+      <c r="AL33" s="74"/>
+      <c r="AM33" s="74"/>
+    </row>
+    <row r="34" spans="29:39" x14ac:dyDescent="0.25">
+      <c r="AC34" s="74"/>
+      <c r="AD34" s="74"/>
+      <c r="AE34" s="74"/>
+      <c r="AG34" s="74"/>
+      <c r="AH34" s="74"/>
+      <c r="AI34" s="74"/>
+      <c r="AK34" s="74"/>
+      <c r="AL34" s="74"/>
+      <c r="AM34" s="74"/>
+    </row>
+    <row r="36" spans="29:39" x14ac:dyDescent="0.25">
+      <c r="AC36" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="AC26" s="76"/>
-      <c r="AD26" s="76"/>
-      <c r="AE26" s="76"/>
-      <c r="AG26" s="76"/>
-      <c r="AH26" s="76"/>
-      <c r="AI26" s="76"/>
-      <c r="AK26" s="76"/>
-      <c r="AL26" s="76"/>
-      <c r="AM26" s="76"/>
-    </row>
-    <row r="27" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC27" s="76"/>
-      <c r="AD27" s="76"/>
-      <c r="AE27" s="76"/>
-      <c r="AG27" s="76"/>
-      <c r="AH27" s="76"/>
-      <c r="AI27" s="76"/>
-      <c r="AK27" s="76"/>
-      <c r="AL27" s="76"/>
-      <c r="AM27" s="76"/>
-    </row>
-    <row r="28" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC28" s="76"/>
-      <c r="AD28" s="76"/>
-      <c r="AE28" s="76"/>
-      <c r="AG28" s="76"/>
-      <c r="AH28" s="76"/>
-      <c r="AI28" s="76"/>
-      <c r="AK28" s="76"/>
-      <c r="AL28" s="76"/>
-      <c r="AM28" s="76"/>
-    </row>
-    <row r="29" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC29" s="76"/>
-      <c r="AD29" s="76"/>
-      <c r="AE29" s="76"/>
-      <c r="AG29" s="76"/>
-      <c r="AH29" s="76"/>
-      <c r="AI29" s="76"/>
-      <c r="AK29" s="76"/>
-      <c r="AL29" s="76"/>
-      <c r="AM29" s="76"/>
-    </row>
-    <row r="30" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC30" s="76"/>
-      <c r="AD30" s="76"/>
-      <c r="AE30" s="76"/>
-      <c r="AG30" s="76"/>
-      <c r="AH30" s="76"/>
-      <c r="AI30" s="76"/>
-      <c r="AK30" s="76"/>
-      <c r="AL30" s="76"/>
-      <c r="AM30" s="76"/>
-    </row>
-    <row r="31" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC31" s="76"/>
-      <c r="AD31" s="76"/>
-      <c r="AE31" s="76"/>
-      <c r="AG31" s="76"/>
-      <c r="AH31" s="76"/>
-      <c r="AI31" s="76"/>
-      <c r="AK31" s="76"/>
-      <c r="AL31" s="76"/>
-      <c r="AM31" s="76"/>
-    </row>
-    <row r="32" spans="15:39" x14ac:dyDescent="0.25">
-      <c r="AC32" s="76"/>
-      <c r="AD32" s="76"/>
-      <c r="AE32" s="76"/>
-      <c r="AG32" s="76"/>
-      <c r="AH32" s="76"/>
-      <c r="AI32" s="76"/>
-      <c r="AK32" s="76"/>
-      <c r="AL32" s="76"/>
-      <c r="AM32" s="76"/>
-    </row>
-    <row r="33" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC33" s="76"/>
-      <c r="AD33" s="76"/>
-      <c r="AE33" s="76"/>
-      <c r="AG33" s="76"/>
-      <c r="AH33" s="76"/>
-      <c r="AI33" s="76"/>
-      <c r="AK33" s="76"/>
-      <c r="AL33" s="76"/>
-      <c r="AM33" s="76"/>
-    </row>
-    <row r="34" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC34" s="76"/>
-      <c r="AD34" s="76"/>
-      <c r="AE34" s="76"/>
-      <c r="AG34" s="76"/>
-      <c r="AH34" s="76"/>
-      <c r="AI34" s="76"/>
-      <c r="AK34" s="76"/>
-      <c r="AL34" s="76"/>
-      <c r="AM34" s="76"/>
-    </row>
-    <row r="36" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC36" s="76" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD36" s="76"/>
-      <c r="AE36" s="76"/>
+      <c r="AD36" s="74"/>
+      <c r="AE36" s="74"/>
     </row>
     <row r="37" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC37" s="76"/>
-      <c r="AD37" s="76"/>
-      <c r="AE37" s="76"/>
+      <c r="AC37" s="74"/>
+      <c r="AD37" s="74"/>
+      <c r="AE37" s="74"/>
     </row>
     <row r="38" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC38" s="76"/>
-      <c r="AD38" s="76"/>
-      <c r="AE38" s="76"/>
+      <c r="AC38" s="74"/>
+      <c r="AD38" s="74"/>
+      <c r="AE38" s="74"/>
     </row>
     <row r="39" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC39" s="76"/>
-      <c r="AD39" s="76"/>
-      <c r="AE39" s="76"/>
+      <c r="AC39" s="74"/>
+      <c r="AD39" s="74"/>
+      <c r="AE39" s="74"/>
     </row>
     <row r="40" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC40" s="76"/>
-      <c r="AD40" s="76"/>
-      <c r="AE40" s="76"/>
+      <c r="AC40" s="74"/>
+      <c r="AD40" s="74"/>
+      <c r="AE40" s="74"/>
     </row>
     <row r="41" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC41" s="76"/>
-      <c r="AD41" s="76"/>
-      <c r="AE41" s="76"/>
+      <c r="AC41" s="74"/>
+      <c r="AD41" s="74"/>
+      <c r="AE41" s="74"/>
     </row>
     <row r="42" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC42" s="76"/>
-      <c r="AD42" s="76"/>
-      <c r="AE42" s="76"/>
+      <c r="AC42" s="74"/>
+      <c r="AD42" s="74"/>
+      <c r="AE42" s="74"/>
     </row>
     <row r="43" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC43" s="76"/>
-      <c r="AD43" s="76"/>
-      <c r="AE43" s="76"/>
+      <c r="AC43" s="74"/>
+      <c r="AD43" s="74"/>
+      <c r="AE43" s="74"/>
     </row>
     <row r="44" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC44" s="76"/>
-      <c r="AD44" s="76"/>
-      <c r="AE44" s="76"/>
+      <c r="AC44" s="74"/>
+      <c r="AD44" s="74"/>
+      <c r="AE44" s="74"/>
     </row>
     <row r="45" spans="29:39" x14ac:dyDescent="0.25">
-      <c r="AC45" s="76"/>
-      <c r="AD45" s="76"/>
-      <c r="AE45" s="76"/>
+      <c r="AC45" s="74"/>
+      <c r="AD45" s="74"/>
+      <c r="AE45" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A15"/>
+    <mergeCell ref="C15:M16"/>
+    <mergeCell ref="AK14:AM23"/>
+    <mergeCell ref="AK25:AM34"/>
+    <mergeCell ref="AK3:AM12"/>
     <mergeCell ref="AC36:AE45"/>
     <mergeCell ref="AC3:AE12"/>
     <mergeCell ref="AG3:AI12"/>
@@ -1904,11 +1912,6 @@
     <mergeCell ref="AG14:AI23"/>
     <mergeCell ref="AC25:AE34"/>
     <mergeCell ref="AG25:AI34"/>
-    <mergeCell ref="A1:A15"/>
-    <mergeCell ref="C15:M16"/>
-    <mergeCell ref="AK14:AM23"/>
-    <mergeCell ref="AK25:AM34"/>
-    <mergeCell ref="AK3:AM12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>